<commit_message>
Topologia frissites, excel frissites
</commit_message>
<xml_diff>
--- a/Vizsgaremek_IPk,VLANok.xlsx
+++ b/Vizsgaremek_IPk,VLANok.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leven\Desktop\Vizsgaremek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leven\Desktop\Vizsgaremek\Dokumentumok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4DD6A7-519F-4C6B-A612-042F73AE6013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7701B68D-B64C-48BF-A7A7-27FABAD4285D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9314BD3E-6A54-4CE4-9518-07F277740BAE}"/>
+    <workbookView xWindow="5415" yWindow="1155" windowWidth="16770" windowHeight="12480" activeTab="3" xr2:uid="{9314BD3E-6A54-4CE4-9518-07F277740BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Szinek" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>#0055ff</t>
   </si>
@@ -270,13 +270,22 @@
   </si>
   <si>
     <t>50.0.0.28/30</t>
+  </si>
+  <si>
+    <t>WIFI</t>
+  </si>
+  <si>
+    <t>DFV_WIFI</t>
+  </si>
+  <si>
+    <t>dfv@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +325,15 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -774,10 +792,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -841,144 +860,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1304,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D835BEC-11F0-4193-810B-6C00DA773C0B}">
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1315,11 +1336,11 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1395,11 +1416,11 @@
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="35"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
       <c r="K12" t="s">
         <v>16</v>
       </c>
@@ -1424,216 +1445,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8310CD62-0451-41AD-9D03-C8EDE9F552C0}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="62"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="53"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="65"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="56"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="55"/>
-      <c r="D7" s="46" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="47"/>
+      <c r="E7" s="58"/>
       <c r="F7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="68" t="s">
+      <c r="H7" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="40" t="s">
+      <c r="I7" s="62"/>
+      <c r="J7" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="41"/>
+      <c r="K7" s="50"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="56"/>
-      <c r="C8" s="57"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="66" t="s">
+      <c r="D9" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="67"/>
+      <c r="E9" s="60"/>
       <c r="F9" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="76" t="s">
+      <c r="J9" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="76"/>
+      <c r="K9" s="40"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="28"/>
       <c r="E10" s="29"/>
-      <c r="J10" s="76" t="s">
+      <c r="J10" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="76"/>
+      <c r="K10" s="40"/>
     </row>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="67"/>
+      <c r="E11" s="60"/>
       <c r="F11" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="76" t="s">
+      <c r="J11" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="76"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
-      <c r="J12" s="76" t="s">
+      <c r="J12" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="76"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="37"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="76" t="s">
+      <c r="J13" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="76"/>
+      <c r="K13" s="40"/>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J14" s="76" t="s">
+      <c r="J14" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="K14" s="76"/>
+      <c r="K14" s="40"/>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="40" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="J15" s="76" t="s">
+      <c r="E15" s="50"/>
+      <c r="J15" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="K15" s="76"/>
+      <c r="K15" s="40"/>
     </row>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J16" s="76" t="s">
+      <c r="J16" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="76"/>
+      <c r="K16" s="40"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="40" t="s">
+      <c r="C17" s="64"/>
+      <c r="D17" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="50"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="40" t="s">
+      <c r="C19" s="66"/>
+      <c r="D19" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="50"/>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="40" t="s">
+      <c r="C21" s="68"/>
+      <c r="D21" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="50"/>
     </row>
     <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40" t="s">
+      <c r="C23" s="70"/>
+      <c r="D23" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="50"/>
     </row>
     <row r="24" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="40" t="s">
+      <c r="C25" s="72"/>
+      <c r="D25" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="41"/>
+      <c r="E25" s="50"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="45"/>
-      <c r="D27" s="46" t="s">
+      <c r="C27" s="74"/>
+      <c r="D27" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="47"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="30" t="s">
         <v>67</v>
       </c>
@@ -1643,40 +1664,16 @@
       <c r="E28" s="32"/>
     </row>
     <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="30" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B3:M4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:E23"/>
@@ -1684,6 +1681,30 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B3:M4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1695,7 +1716,7 @@
   <dimension ref="B1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,20 +1728,20 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="63"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="65"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1799,20 +1820,20 @@
       <c r="E13" s="18"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="79" t="s">
+      <c r="E14" s="35" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="25" t="s">
@@ -1835,10 +1856,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E59B741-2061-4745-830D-5CC374750031}">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,22 +1871,22 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="73"/>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="75"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1889,10 +1910,10 @@
       <c r="D7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="76"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1904,10 +1925,21 @@
       <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="76"/>
+      <c r="F8" s="40"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="81" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1915,6 +1947,9 @@
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{18DA9C9D-CA39-46EA-9639-E07F64F4C2D0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
dokumentacio javitasa, excel bovitese, tesztelesi bovitese
</commit_message>
<xml_diff>
--- a/Vizsgaremek_IPk,VLANok.xlsx
+++ b/Vizsgaremek_IPk,VLANok.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leven\Desktop\GitHub\VizsgaremekCsapat2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\VizsgaremekCsapat2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CF7694-2F85-4B1E-AC0C-34DE406AF60D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A69FC0-72C7-446A-8710-9558501EB2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{9314BD3E-6A54-4CE4-9518-07F277740BAE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9314BD3E-6A54-4CE4-9518-07F277740BAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Szinek" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="161">
   <si>
     <t>#0055ff</t>
   </si>
@@ -495,6 +494,33 @@
   </si>
   <si>
     <t>2010:2010:B::/64</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>SSH</t>
+  </si>
+  <si>
+    <t>vajdaadmin</t>
+  </si>
+  <si>
+    <t>vajda1234</t>
+  </si>
+  <si>
+    <t>Mindenhol</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Isakmp</t>
+  </si>
+  <si>
+    <t>VPN</t>
+  </si>
+  <si>
+    <t>vajdavpnpa55</t>
   </si>
 </sst>
 </file>
@@ -1144,6 +1170,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1162,26 +1194,92 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1189,89 +1287,17 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1619,7 +1645,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1629,8 +1655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D835BEC-11F0-4193-810B-6C00DA773C0B}">
   <dimension ref="B1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8310CD62-0451-41AD-9D03-C8EDE9F552C0}">
   <dimension ref="B2:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,188 +1808,188 @@
   <sheetData>
     <row r="2" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="59"/>
-      <c r="O3" s="57" t="s">
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="61"/>
+      <c r="O3" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="59"/>
-      <c r="T3" s="57" t="s">
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="61"/>
+      <c r="T3" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="59"/>
-      <c r="AG3" s="57" t="s">
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="61"/>
+      <c r="AG3" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58"/>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="58"/>
-      <c r="AN3" s="58"/>
-      <c r="AO3" s="58"/>
-      <c r="AP3" s="59"/>
+      <c r="AH3" s="60"/>
+      <c r="AI3" s="60"/>
+      <c r="AJ3" s="60"/>
+      <c r="AK3" s="60"/>
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="60"/>
+      <c r="AN3" s="60"/>
+      <c r="AO3" s="60"/>
+      <c r="AP3" s="61"/>
     </row>
     <row r="4" spans="2:42" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="60"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="62"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="R4" s="62"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="61"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="61"/>
-      <c r="AA4" s="61"/>
-      <c r="AB4" s="61"/>
-      <c r="AC4" s="61"/>
-      <c r="AD4" s="61"/>
-      <c r="AE4" s="62"/>
-      <c r="AG4" s="60"/>
-      <c r="AH4" s="61"/>
-      <c r="AI4" s="61"/>
-      <c r="AJ4" s="61"/>
-      <c r="AK4" s="61"/>
-      <c r="AL4" s="61"/>
-      <c r="AM4" s="61"/>
-      <c r="AN4" s="61"/>
-      <c r="AO4" s="61"/>
-      <c r="AP4" s="62"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="64"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="63"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="63"/>
+      <c r="Z4" s="63"/>
+      <c r="AA4" s="63"/>
+      <c r="AB4" s="63"/>
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="63"/>
+      <c r="AE4" s="64"/>
+      <c r="AG4" s="62"/>
+      <c r="AH4" s="63"/>
+      <c r="AI4" s="63"/>
+      <c r="AJ4" s="63"/>
+      <c r="AK4" s="63"/>
+      <c r="AL4" s="63"/>
+      <c r="AM4" s="63"/>
+      <c r="AN4" s="63"/>
+      <c r="AO4" s="63"/>
+      <c r="AP4" s="64"/>
     </row>
     <row r="5" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O6" s="65" t="s">
+      <c r="O6" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="94" t="s">
+      <c r="P6" s="58"/>
+      <c r="Q6" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="R6" s="66"/>
-      <c r="U6" s="76" t="s">
+      <c r="R6" s="58"/>
+      <c r="U6" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="V6" s="77"/>
-      <c r="W6" s="97" t="s">
+      <c r="V6" s="67"/>
+      <c r="W6" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="X6" s="98"/>
+      <c r="X6" s="69"/>
       <c r="Y6" t="s">
         <v>97</v>
       </c>
-      <c r="AH6" s="63" t="s">
+      <c r="AH6" s="97" t="s">
         <v>48</v>
       </c>
-      <c r="AI6" s="64"/>
-      <c r="AJ6" s="65" t="s">
+      <c r="AI6" s="98"/>
+      <c r="AJ6" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="AK6" s="66"/>
+      <c r="AK6" s="58"/>
     </row>
     <row r="7" spans="2:42" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="90" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="72" t="s">
+      <c r="C7" s="91"/>
+      <c r="D7" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="81"/>
       <c r="F7" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="65" t="s">
+      <c r="I7" s="67"/>
+      <c r="J7" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="66"/>
-      <c r="O7" s="65" t="s">
+      <c r="K7" s="58"/>
+      <c r="O7" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="65" t="s">
+      <c r="P7" s="58"/>
+      <c r="Q7" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="R7" s="66"/>
+      <c r="R7" s="58"/>
     </row>
     <row r="8" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="80"/>
-      <c r="C8" s="81"/>
+      <c r="B8" s="92"/>
+      <c r="C8" s="93"/>
       <c r="D8" s="28"/>
       <c r="E8" s="29"/>
-      <c r="Q8" s="68" t="s">
+      <c r="Q8" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="R8" s="68"/>
-      <c r="U8" s="76" t="s">
+      <c r="R8" s="73"/>
+      <c r="U8" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="V8" s="77"/>
-      <c r="W8" s="99" t="s">
+      <c r="V8" s="67"/>
+      <c r="W8" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="X8" s="98"/>
+      <c r="X8" s="69"/>
       <c r="Y8" t="s">
         <v>98</v>
       </c>
       <c r="AA8" s="56"/>
       <c r="AB8" s="56"/>
-      <c r="AH8" s="63" t="s">
+      <c r="AH8" s="97" t="s">
         <v>119</v>
       </c>
-      <c r="AI8" s="64"/>
-      <c r="AJ8" s="65" t="s">
+      <c r="AI8" s="98"/>
+      <c r="AJ8" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="AK8" s="66"/>
+      <c r="AK8" s="58"/>
     </row>
     <row r="9" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="75"/>
+      <c r="E9" s="89"/>
       <c r="F9" s="30" t="s">
         <v>21</v>
       </c>
@@ -1989,25 +2015,25 @@
       <c r="Y10" t="s">
         <v>104</v>
       </c>
-      <c r="AA10" s="65" t="s">
+      <c r="AA10" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="AB10" s="66"/>
-      <c r="AH10" s="63" t="s">
+      <c r="AB10" s="58"/>
+      <c r="AH10" s="97" t="s">
         <v>125</v>
       </c>
-      <c r="AI10" s="67"/>
-      <c r="AJ10" s="64"/>
-      <c r="AK10" s="65" t="s">
+      <c r="AI10" s="99"/>
+      <c r="AJ10" s="98"/>
+      <c r="AK10" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="AL10" s="66"/>
+      <c r="AL10" s="58"/>
     </row>
     <row r="11" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="88" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="75"/>
+      <c r="E11" s="89"/>
       <c r="F11" s="30" t="s">
         <v>32</v>
       </c>
@@ -2023,37 +2049,37 @@
         <v>72</v>
       </c>
       <c r="K12" s="56"/>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
-      <c r="R12" s="59"/>
-      <c r="U12" s="65" t="s">
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="61"/>
+      <c r="U12" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="V12" s="66"/>
-      <c r="W12" s="65" t="s">
+      <c r="V12" s="58"/>
+      <c r="W12" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="X12" s="66"/>
-      <c r="AA12" s="65" t="s">
+      <c r="X12" s="58"/>
+      <c r="AA12" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="AB12" s="66"/>
+      <c r="AB12" s="58"/>
       <c r="AH12" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="AI12" s="65" t="s">
+      <c r="AI12" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="AJ12" s="66"/>
+      <c r="AJ12" s="58"/>
     </row>
     <row r="13" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="95" t="s">
+      <c r="D13" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="96"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="30" t="s">
         <v>46</v>
       </c>
@@ -2061,10 +2087,10 @@
         <v>73</v>
       </c>
       <c r="K13" s="56"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="64"/>
     </row>
     <row r="14" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J14" s="56" t="s">
@@ -2081,50 +2107,50 @@
       <c r="AK14" s="56"/>
     </row>
     <row r="15" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="65" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="66"/>
+      <c r="E15" s="58"/>
       <c r="J15" s="56" t="s">
         <v>75</v>
       </c>
       <c r="K15" s="56"/>
-      <c r="O15" s="65" t="s">
+      <c r="O15" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="94" t="s">
+      <c r="P15" s="58"/>
+      <c r="Q15" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="66"/>
+      <c r="R15" s="58"/>
     </row>
     <row r="16" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J16" s="56" t="s">
         <v>76</v>
       </c>
       <c r="K16" s="56"/>
-      <c r="O16" s="65" t="s">
+      <c r="O16" s="57" t="s">
         <v>114</v>
       </c>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="65" t="s">
+      <c r="P16" s="58"/>
+      <c r="Q16" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="R16" s="66"/>
+      <c r="R16" s="58"/>
     </row>
     <row r="17" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="82" t="s">
         <v>52</v>
       </c>
       <c r="C17" s="83"/>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="66"/>
+      <c r="E17" s="58"/>
       <c r="H17" s="56" t="s">
         <v>136</v>
       </c>
@@ -2133,10 +2159,10 @@
         <v>135</v>
       </c>
       <c r="K17" s="56"/>
-      <c r="Q17" s="68" t="s">
+      <c r="Q17" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="R17" s="68"/>
+      <c r="R17" s="73"/>
     </row>
     <row r="18" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H18" s="56" t="s">
@@ -2153,10 +2179,10 @@
         <v>54</v>
       </c>
       <c r="C19" s="85"/>
-      <c r="D19" s="65" t="s">
+      <c r="D19" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="66"/>
+      <c r="E19" s="58"/>
     </row>
     <row r="20" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2164,98 +2190,98 @@
         <v>49</v>
       </c>
       <c r="C21" s="87"/>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="66"/>
-      <c r="O21" s="57" t="s">
+      <c r="E21" s="58"/>
+      <c r="O21" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="59"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="R21" s="61"/>
     </row>
     <row r="22" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O22" s="60"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="62"/>
+      <c r="O22" s="62"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="64"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="89"/>
-      <c r="D23" s="65" t="s">
+      <c r="C23" s="75"/>
+      <c r="D23" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="66"/>
+      <c r="E23" s="58"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O24" s="65" t="s">
+      <c r="O24" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="P24" s="66"/>
-      <c r="Q24" s="69" t="s">
+      <c r="P24" s="58"/>
+      <c r="Q24" s="96" t="s">
         <v>149</v>
       </c>
       <c r="R24" s="56"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="91"/>
-      <c r="D25" s="65" t="s">
+      <c r="C25" s="77"/>
+      <c r="D25" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="66"/>
-      <c r="F25" s="65" t="s">
+      <c r="E25" s="58"/>
+      <c r="F25" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="66"/>
-      <c r="O25" s="65" t="s">
+      <c r="G25" s="58"/>
+      <c r="O25" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="P25" s="66"/>
+      <c r="P25" s="58"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="2:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="92" t="s">
+      <c r="B27" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="72" t="s">
+      <c r="C27" s="79"/>
+      <c r="D27" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="73"/>
+      <c r="E27" s="81"/>
       <c r="F27" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="N27" s="57" t="s">
+      <c r="N27" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="59"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="61"/>
     </row>
     <row r="28" spans="2:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="31"/>
       <c r="E28" s="32"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
-      <c r="R28" s="61"/>
-      <c r="S28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="63"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="63"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="64"/>
     </row>
     <row r="29" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="95" t="s">
+      <c r="D29" s="71" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="96"/>
+      <c r="E29" s="72"/>
       <c r="F29" s="30" t="s">
         <v>46</v>
       </c>
@@ -2310,72 +2336,6 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="W14:X14"/>
-    <mergeCell ref="W12:X12"/>
-    <mergeCell ref="U12:V12"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AI12:AJ12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="O3:R4"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="O12:R13"/>
-    <mergeCell ref="T3:AE4"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B3:M4"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="O21:R22"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="Q24:R24"/>
     <mergeCell ref="O36:P36"/>
     <mergeCell ref="O37:P37"/>
     <mergeCell ref="O34:P34"/>
@@ -2392,6 +2352,72 @@
     <mergeCell ref="W10:X10"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="N27:S28"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="O21:R22"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B3:M4"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="O3:R4"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="O12:R13"/>
+    <mergeCell ref="T3:AE4"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="U12:V12"/>
+    <mergeCell ref="AJ14:AK14"/>
+    <mergeCell ref="AI12:AJ12"/>
+    <mergeCell ref="AA12:AB12"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2418,20 +2444,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2464,7 +2490,7 @@
       <c r="J6" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="K6" s="73"/>
+      <c r="K6" s="81"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
@@ -2494,7 +2520,7 @@
       <c r="J8" s="101" t="s">
         <v>124</v>
       </c>
-      <c r="K8" s="75"/>
+      <c r="K8" s="89"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C9" s="16"/>
@@ -2524,7 +2550,7 @@
       <c r="J10" s="102" t="s">
         <v>132</v>
       </c>
-      <c r="K10" s="96"/>
+      <c r="K10" s="72"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C11" s="16"/>
@@ -2631,10 +2657,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E59B741-2061-4745-830D-5CC374750031}">
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2757,6 +2783,42 @@
       </c>
       <c r="E14" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+      <c r="C16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D19" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>